<commit_message>
update IG - resolve FHIR group comments
</commit_message>
<xml_diff>
--- a/v0.7/StructureDefinition-Communication.xlsx
+++ b/v0.7/StructureDefinition-Communication.xlsx
@@ -538,7 +538,7 @@
     <t>Communication.inResponseTo</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Communication)
+    <t xml:space="preserve">Reference(https://ig.hcxprotocol.io/v0.7/StructureDefinition-Communication.html)
 </t>
   </si>
   <si>
@@ -674,7 +674,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Patient|Group)
+    <t xml:space="preserve">Reference(https://nrces.in/ndhm/fhir/r4/StructureDefinition/Patient|Group)
 </t>
   </si>
   <si>
@@ -726,7 +726,7 @@
     <t>Communication.encounter</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Encounter)
+    <t xml:space="preserve">Reference(https://nrces.in/ndhm/fhir/r4/StructureDefinition/Encounter)
 </t>
   </si>
   <si>
@@ -776,7 +776,7 @@
     <t>Communication.recipient</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Device|Organization|Patient|Practitioner|PractitionerRole|RelatedPerson|Group|CareTeam|HealthcareService)
+    <t xml:space="preserve">Reference(Device|https://nrces.in/ndhm/fhir/r4/StructureDefinition/Organization|https://nrces.in/ndhm/fhir/r4/StructureDefinition/Patient|https://nrces.in/ndhm/fhir/r4/StructureDefinition/Practitioner|https://nrces.in/ndhm/fhir/r4/StructureDefinition/PractitionerRole|RelatedPerson|Group|CareTeam|HealthcareService)
 </t>
   </si>
   <si>
@@ -795,7 +795,7 @@
     <t>Communication.sender</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Device|Organization|Patient|Practitioner|PractitionerRole|RelatedPerson|HealthcareService)
+    <t xml:space="preserve">Reference(Device|https://nrces.in/ndhm/fhir/r4/StructureDefinition/Organization|https://nrces.in/ndhm/fhir/r4/StructureDefinition/Patient|https://nrces.in/ndhm/fhir/r4/StructureDefinition/Practitioner|https://nrces.in/ndhm/fhir/r4/StructureDefinition/PractitionerRole|RelatedPerson|HealthcareService)
 </t>
   </si>
   <si>
@@ -835,7 +835,7 @@
     <t>Communication.reasonReference</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Condition|Observation|DiagnosticReport|DocumentReference)
+    <t xml:space="preserve">Reference(https://nrces.in/ndhm/fhir/r4/StructureDefinition/Condition|https://nrces.in/ndhm/fhir/r4/StructureDefinition/Observation|DiagnosticReport|https://nrces.in/ndhm/fhir/r4/StructureDefinition/DocumentReference)
 </t>
   </si>
   <si>
@@ -2371,7 +2371,7 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" t="s" s="2">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="F11" t="s" s="2">
         <v>73</v>

</xml_diff>